<commit_message>
Skill Course Weighting Master
</commit_message>
<xml_diff>
--- a/01_BachelorWifoMannheim/04_Graph/CourseSkillWeights.xlsx
+++ b/01_BachelorWifoMannheim/04_Graph/CourseSkillWeights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Masterarbeit/Course_Suggestion/01_BachelorWifoMannheim/04_Graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2BC950BED3605920531B3611595ED87656CD3BDA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7097CFD-C405-4C7E-B81D-C509B3312482}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2BC950BED3605920531B3611595ED87656CD3BDA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C88B5D83-7264-4204-957A-68E584803486}"/>
   <bookViews>
-    <workbookView xWindow="-27030" yWindow="2415" windowWidth="21600" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
   <si>
     <t>Weight</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>SM 457 Seminar Prof. van der Aa Seminar on Process Analysis</t>
-  </si>
-  <si>
-    <t>BA 450 Bachelor-Abschlussarbeit Bachelor Thesis</t>
   </si>
   <si>
     <t>Grundlagen des externen Rechnungswesens</t>
@@ -620,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:E81"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2031,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2048,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" t="s">
         <v>63</v>
-      </c>
-      <c r="C84" t="s">
-        <v>64</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2068,7 +2065,7 @@
         <v>65</v>
       </c>
       <c r="C85" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -2082,10 +2079,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C86" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2099,10 +2096,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -2113,53 +2110,53 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0</v>
+        <v>27.946998946998921</v>
       </c>
       <c r="B88" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C88" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>770</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>27.946998946998921</v>
+        <v>62.873507728310408</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D89">
-        <v>148</v>
+        <v>1547</v>
       </c>
       <c r="E89">
-        <v>770</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>62.873507728310408</v>
+        <v>0</v>
       </c>
       <c r="B90" t="s">
         <v>74</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D90">
-        <v>1547</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>2686</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,32 +2164,15 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C91" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0</v>
-      </c>
-      <c r="B92" t="s">
-        <v>77</v>
-      </c>
-      <c r="C92" t="s">
-        <v>78</v>
-      </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-      <c r="E92">
         <v>0</v>
       </c>
     </row>

</xml_diff>